<commit_message>
[Vinay] created a voucher bill payment feature
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/financialTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/financialTestData.xlsx
@@ -20,9 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t xml:space="preserve">dataName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">voucherDate</t>
   </si>
   <si>
     <t xml:space="preserve">voucherType</t>
@@ -95,6 +98,9 @@
   </si>
   <si>
     <t xml:space="preserve">Public Health</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30/06/2016</t>
   </si>
 </sst>
 </file>
@@ -209,81 +215,108 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.9740740740741"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.937037037037"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="14.5037037037037"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="16.0703703703704"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.4"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.1851851851852"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.62222222222222"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.8"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.2296296296296"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.2296296296296"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="14.7962962962963"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="16.462962962963"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.0851851851852"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.7740740740741"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.81851851851852"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="0" t="s">
         <v>5</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="17.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="1" t="n">
+      <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1" t="n">
         <v>3501001</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>9</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>10</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="1" t="n">
+      <c r="C3" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="1" t="n">
         <v>2101001</v>
       </c>
-      <c r="D3" s="1" t="n">
+      <c r="E3" s="1" t="n">
         <v>3501003</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>13</v>
       </c>
       <c r="F3" s="0" t="s">
         <v>14</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="18.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>2101001</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>3501003</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Vinay] Modified the financial fetures
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/financialTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/financialTestData.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="journalVoucherDetails" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="financialBankDetails" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
   <si>
     <t xml:space="preserve">dataName</t>
   </si>
@@ -44,6 +45,9 @@
   </si>
   <si>
     <t xml:space="preserve">voucher1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27/12/2016</t>
   </si>
   <si>
     <t xml:space="preserve">General</t>
@@ -100,7 +104,25 @@
     <t xml:space="preserve">Public Health</t>
   </si>
   <si>
+    <t xml:space="preserve">voucherDateJune</t>
+  </si>
+  <si>
     <t xml:space="preserve">30/06/2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bankName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">accountNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SBI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANDHRA BANK-Andhra Bank RTC Busstand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4502110--110710100009664--ANDHRA BANK</t>
   </si>
 </sst>
 </file>
@@ -217,20 +239,20 @@
   </sheetPr>
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.8"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.2296296296296"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.2296296296296"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="14.7962962962963"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="16.462962962963"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.0851851851852"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.7740740740741"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.81851851851852"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.2333333333333"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.1111111111111"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.1111111111111"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="15.8740740740741"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="17.6407407407407"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="32.337037037037"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.7333333333333"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.40740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -260,28 +282,34 @@
       <c r="A2" s="0" t="s">
         <v>7</v>
       </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="C2" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E2" s="1" t="n">
         <v>3501001</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>2101001</v>
@@ -290,21 +318,21 @@
         <v>3501003</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="18.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>2101001</v>
@@ -313,10 +341,62 @@
         <v>3501003</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.2888888888889"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.5111111111111"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="48.9"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.62222222222222"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="16.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[PHOENIX-5869] Completed the bill payment of voucher
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/financialTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/financialTestData.xlsx
@@ -120,10 +120,10 @@
     <t xml:space="preserve">SBI</t>
   </si>
   <si>
-    <t xml:space="preserve">STATE BANK OF INDIA-SBI Tresury Branch, Kurnool</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4502106--844810206002--STATE BANK OF INDIA</t>
+    <t xml:space="preserve">KOTAK MAHINDRA BANK-Ucon Plaza Kurnool</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4502205--311010192115--KOTAK MAHINDRA BANK</t>
   </si>
   <si>
     <t xml:space="preserve">fund</t>
@@ -395,7 +395,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
[PHOENIX-5928] Compelted the creation of journal voucher with budget check
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/financialTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/financialTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="journalVoucherDetails" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
   <si>
     <t xml:space="preserve">dataName</t>
   </si>
@@ -109,6 +109,24 @@
   </si>
   <si>
     <t xml:space="preserve">30/06/2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">budgetCheck</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03/01/2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2101001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3501003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ENGINEERING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Water Supply</t>
   </si>
   <si>
     <t xml:space="preserve">bankName</t>
@@ -266,22 +284,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.6407407407407"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.3851851851852"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.3851851851852"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="17.3444444444444"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="19.2074074074074"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="35.5703703703704"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.5740740740741"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.1925925925926"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.0296296296296"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.7777777777778"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.7777777777778"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="17.737037037037"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="19.6962962962963"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="36.4555555555556"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.3592592592593"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.3888888888889"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -374,6 +392,29 @@
       </c>
       <c r="G4" s="0" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -394,16 +435,16 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.2703703703704"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.5296296296296"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="53.8962962962963"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.40740740740741"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.562962962963"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.5111111111111"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="55.2703703703704"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.6037037037037"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -411,21 +452,21 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -452,14 +493,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.662962962963"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.3074074074074"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.3777777777778"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="25.1851851851852"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.6592592592593"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="17.3444444444444"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="18.3259259259259"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.62222222222222"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.9555555555556"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.6"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.162962962963"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="25.7740740740741"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.0518518518519"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="17.737037037037"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="18.7185185185185"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.81851851851852"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -467,7 +508,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>5</v>
@@ -476,30 +517,30 @@
         <v>6</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>15</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="F2" s="1" t="n">
         <v>2101009</v>

</xml_diff>

<commit_message>
[PHOENIX-5941] Compelted the creation of the remittance recovery
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/financialTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/financialTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="journalVoucherDetails" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="42">
   <si>
     <t xml:space="preserve">dataName</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t xml:space="preserve">function</t>
+  </si>
+  <si>
+    <t xml:space="preserve">accountCode3</t>
   </si>
   <si>
     <t xml:space="preserve">voucher1</t>
@@ -129,6 +132,9 @@
     <t xml:space="preserve">Water Supply</t>
   </si>
   <si>
+    <t xml:space="preserve">remittance</t>
+  </si>
+  <si>
     <t xml:space="preserve">bankName</t>
   </si>
   <si>
@@ -142,6 +148,12 @@
   </si>
   <si>
     <t xml:space="preserve">4502205--311010192115--KOTAK MAHINDRA BANK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SBI1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KOTAK MAHINDRA BANK Ucon Plaza Kurnool</t>
   </si>
   <si>
     <t xml:space="preserve">fund</t>
@@ -284,10 +296,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H6" activeCellId="0" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -298,8 +310,9 @@
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="17.737037037037"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="19.6962962962963"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="36.4555555555556"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.3592592592593"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.3888888888889"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.3037037037037"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.5407407407407"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.3888888888889"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -324,39 +337,42 @@
       <c r="G1" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="17.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E2" s="1" t="n">
         <v>3501001</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>2101001</v>
@@ -365,21 +381,21 @@
         <v>3501003</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="18.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>2101001</v>
@@ -388,33 +404,59 @@
         <v>3501003</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="C6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="0" t="s">
+      <c r="E6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="0" t="s">
-        <v>24</v>
+      <c r="F6" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>3502002</v>
       </c>
     </row>
   </sheetData>
@@ -433,10 +475,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -452,21 +494,32 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -508,7 +561,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>5</v>
@@ -517,30 +570,30 @@
         <v>6</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="F2" s="1" t="n">
         <v>2101009</v>

</xml_diff>

<commit_message>
[PHOENIX-6105] Completed the cheque/RTGS assignment scenario
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/financialTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/financialTestData.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="journalVoucherDetails" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="financialBankDetails" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="financialExpenseBillDetails" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="experiment" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="44">
   <si>
     <t xml:space="preserve">dataName</t>
   </si>
@@ -181,6 +182,9 @@
   </si>
   <si>
     <t xml:space="preserve">Contingent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">number</t>
   </si>
 </sst>
 </file>
@@ -265,7 +269,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -279,6 +283,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -301,21 +309,21 @@
   </sheetPr>
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.4222222222222"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.1703703703704"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.1703703703704"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.1296296296296"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="20.1851851851852"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="37.4333333333333"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.8888888888889"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.8555555555556"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.5851851851852"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.8148148148148"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.5592592592593"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.5592592592593"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.5222222222222"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="20.6777777777778"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="38.3148148148148"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.4777777777778"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.2481481481481"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.7777777777778"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -481,15 +489,15 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.8555555555556"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="44.5888888888889"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="56.6407407407407"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.8"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.1518518518519"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="45.6666666666667"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="58.0111111111111"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.9962962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -549,14 +557,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.2481481481481"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.8962962962963"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.9444444444444"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="26.4592592592593"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.3444444444444"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="18.1296296296296"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="19.1074074074074"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.4444444444444"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.2888888888889"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.6333333333333"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="27.1444444444444"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.737037037037"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="18.5222222222222"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="19.5"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.21111111111111"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -603,6 +611,1019 @@
       </c>
       <c r="G2" s="1" t="n">
         <v>3501102</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B123"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.61111111111111"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.49259259259259"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36296296296296"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="20.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="n">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="n">
+        <v>100001</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="n">
+        <v>100002</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="n">
+        <v>100003</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="n">
+        <v>100004</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="n">
+        <v>100005</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4" t="n">
+        <v>100006</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4" t="n">
+        <v>100007</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4" t="n">
+        <v>100008</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4" t="n">
+        <v>100009</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4" t="n">
+        <v>100010</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4" t="n">
+        <v>100011</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="4" t="n">
+        <v>100012</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="4" t="n">
+        <v>100013</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="4" t="n">
+        <v>100014</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="4" t="n">
+        <v>100015</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="4" t="n">
+        <v>100016</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="4" t="n">
+        <v>100017</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="4" t="n">
+        <v>100018</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="4" t="n">
+        <v>100019</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="4" t="n">
+        <v>100020</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="4" t="n">
+        <v>100021</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="4" t="n">
+        <v>100022</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="4" t="n">
+        <v>100023</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="4" t="n">
+        <v>100024</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="4" t="n">
+        <v>100025</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="4" t="n">
+        <v>100026</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="4" t="n">
+        <v>100027</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="4" t="n">
+        <v>100028</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="4" t="n">
+        <v>100029</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="4" t="n">
+        <v>100030</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="4" t="n">
+        <v>100031</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="4" t="n">
+        <v>100032</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="4" t="n">
+        <v>100033</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="4" t="n">
+        <v>100034</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="4" t="n">
+        <v>100035</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="4" t="n">
+        <v>100036</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="4" t="n">
+        <v>100037</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="4" t="n">
+        <v>100038</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="4" t="n">
+        <v>100039</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" s="4" t="n">
+        <v>100040</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" s="4" t="n">
+        <v>100041</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" s="4" t="n">
+        <v>100042</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" s="4" t="n">
+        <v>100043</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" s="4" t="n">
+        <v>100044</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" s="4" t="n">
+        <v>100045</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" s="4" t="n">
+        <v>100046</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" s="4" t="n">
+        <v>100047</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" s="4" t="n">
+        <v>100048</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" s="4" t="n">
+        <v>100049</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="n">
+        <v>51</v>
+      </c>
+      <c r="B52" s="4" t="n">
+        <v>100050</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="n">
+        <v>52</v>
+      </c>
+      <c r="B53" s="4" t="n">
+        <v>100051</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="n">
+        <v>53</v>
+      </c>
+      <c r="B54" s="4" t="n">
+        <v>100052</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="n">
+        <v>54</v>
+      </c>
+      <c r="B55" s="4" t="n">
+        <v>100053</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="n">
+        <v>55</v>
+      </c>
+      <c r="B56" s="4" t="n">
+        <v>100054</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="n">
+        <v>56</v>
+      </c>
+      <c r="B57" s="4" t="n">
+        <v>100055</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="n">
+        <v>57</v>
+      </c>
+      <c r="B58" s="4" t="n">
+        <v>100056</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="n">
+        <v>58</v>
+      </c>
+      <c r="B59" s="4" t="n">
+        <v>100057</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="n">
+        <v>59</v>
+      </c>
+      <c r="B60" s="4" t="n">
+        <v>100058</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="B61" s="4" t="n">
+        <v>100059</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="n">
+        <v>61</v>
+      </c>
+      <c r="B62" s="4" t="n">
+        <v>100060</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0" t="n">
+        <v>62</v>
+      </c>
+      <c r="B63" s="4" t="n">
+        <v>100061</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0" t="n">
+        <v>63</v>
+      </c>
+      <c r="B64" s="4" t="n">
+        <v>100062</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="n">
+        <v>64</v>
+      </c>
+      <c r="B65" s="4" t="n">
+        <v>100063</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="0" t="n">
+        <v>65</v>
+      </c>
+      <c r="B66" s="4" t="n">
+        <v>100064</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="0" t="n">
+        <v>66</v>
+      </c>
+      <c r="B67" s="4" t="n">
+        <v>100065</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="0" t="n">
+        <v>67</v>
+      </c>
+      <c r="B68" s="4" t="n">
+        <v>100066</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0" t="n">
+        <v>68</v>
+      </c>
+      <c r="B69" s="4" t="n">
+        <v>100067</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="0" t="n">
+        <v>69</v>
+      </c>
+      <c r="B70" s="4" t="n">
+        <v>100068</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="B71" s="4" t="n">
+        <v>100069</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="0" t="n">
+        <v>71</v>
+      </c>
+      <c r="B72" s="4" t="n">
+        <v>100070</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="0" t="n">
+        <v>72</v>
+      </c>
+      <c r="B73" s="4" t="n">
+        <v>100071</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="0" t="n">
+        <v>73</v>
+      </c>
+      <c r="B74" s="4" t="n">
+        <v>100072</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="0" t="n">
+        <v>74</v>
+      </c>
+      <c r="B75" s="4" t="n">
+        <v>100073</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="0" t="n">
+        <v>75</v>
+      </c>
+      <c r="B76" s="4" t="n">
+        <v>100074</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="0" t="n">
+        <v>76</v>
+      </c>
+      <c r="B77" s="4" t="n">
+        <v>100075</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0" t="n">
+        <v>77</v>
+      </c>
+      <c r="B78" s="4" t="n">
+        <v>100076</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="0" t="n">
+        <v>78</v>
+      </c>
+      <c r="B79" s="4" t="n">
+        <v>100077</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="0" t="n">
+        <v>79</v>
+      </c>
+      <c r="B80" s="4" t="n">
+        <v>100078</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="B81" s="4" t="n">
+        <v>100079</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="0" t="n">
+        <v>81</v>
+      </c>
+      <c r="B82" s="4" t="n">
+        <v>100080</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="0" t="n">
+        <v>82</v>
+      </c>
+      <c r="B83" s="4" t="n">
+        <v>100081</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="0" t="n">
+        <v>83</v>
+      </c>
+      <c r="B84" s="4" t="n">
+        <v>100082</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="0" t="n">
+        <v>84</v>
+      </c>
+      <c r="B85" s="4" t="n">
+        <v>100083</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="0" t="n">
+        <v>85</v>
+      </c>
+      <c r="B86" s="4" t="n">
+        <v>100084</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="0" t="n">
+        <v>86</v>
+      </c>
+      <c r="B87" s="4" t="n">
+        <v>100085</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="0" t="n">
+        <v>87</v>
+      </c>
+      <c r="B88" s="4" t="n">
+        <v>100086</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="0" t="n">
+        <v>88</v>
+      </c>
+      <c r="B89" s="4" t="n">
+        <v>100087</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="0" t="n">
+        <v>89</v>
+      </c>
+      <c r="B90" s="4" t="n">
+        <v>100088</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="0" t="n">
+        <v>90</v>
+      </c>
+      <c r="B91" s="4" t="n">
+        <v>100089</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="0" t="n">
+        <v>91</v>
+      </c>
+      <c r="B92" s="4" t="n">
+        <v>100090</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="0" t="n">
+        <v>92</v>
+      </c>
+      <c r="B93" s="4" t="n">
+        <v>100091</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="B94" s="4" t="n">
+        <v>100092</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="0" t="n">
+        <v>94</v>
+      </c>
+      <c r="B95" s="4" t="n">
+        <v>100093</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="0" t="n">
+        <v>95</v>
+      </c>
+      <c r="B96" s="4" t="n">
+        <v>100094</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="0" t="n">
+        <v>96</v>
+      </c>
+      <c r="B97" s="4" t="n">
+        <v>100095</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="0" t="n">
+        <v>97</v>
+      </c>
+      <c r="B98" s="4" t="n">
+        <v>100096</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="0" t="n">
+        <v>98</v>
+      </c>
+      <c r="B99" s="4" t="n">
+        <v>100097</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="0" t="n">
+        <v>99</v>
+      </c>
+      <c r="B100" s="4" t="n">
+        <v>100098</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="B101" s="4" t="n">
+        <v>100099</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="0" t="n">
+        <v>101</v>
+      </c>
+      <c r="B102" s="4" t="n">
+        <v>100100</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="0" t="n">
+        <v>102</v>
+      </c>
+      <c r="B103" s="4" t="n">
+        <v>100101</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="0" t="n">
+        <v>103</v>
+      </c>
+      <c r="B104" s="4" t="n">
+        <v>100102</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="0" t="n">
+        <v>104</v>
+      </c>
+      <c r="B105" s="4" t="n">
+        <v>100103</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="0" t="n">
+        <v>105</v>
+      </c>
+      <c r="B106" s="4" t="n">
+        <v>100104</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="0" t="n">
+        <v>106</v>
+      </c>
+      <c r="B107" s="4" t="n">
+        <v>100105</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="0" t="n">
+        <v>107</v>
+      </c>
+      <c r="B108" s="4" t="n">
+        <v>100106</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="0" t="n">
+        <v>108</v>
+      </c>
+      <c r="B109" s="4" t="n">
+        <v>100107</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="0" t="n">
+        <v>109</v>
+      </c>
+      <c r="B110" s="4" t="n">
+        <v>100108</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="0" t="n">
+        <v>110</v>
+      </c>
+      <c r="B111" s="4" t="n">
+        <v>100109</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="0" t="n">
+        <v>111</v>
+      </c>
+      <c r="B112" s="4" t="n">
+        <v>100110</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="0" t="n">
+        <v>112</v>
+      </c>
+      <c r="B113" s="4" t="n">
+        <v>100111</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="0" t="n">
+        <v>113</v>
+      </c>
+      <c r="B114" s="4" t="n">
+        <v>100112</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="0" t="n">
+        <v>114</v>
+      </c>
+      <c r="B115" s="4" t="n">
+        <v>100113</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="0" t="n">
+        <v>115</v>
+      </c>
+      <c r="B116" s="4" t="n">
+        <v>100114</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="0" t="n">
+        <v>116</v>
+      </c>
+      <c r="B117" s="4" t="n">
+        <v>100115</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="0" t="n">
+        <v>117</v>
+      </c>
+      <c r="B118" s="4" t="n">
+        <v>100116</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="0" t="n">
+        <v>118</v>
+      </c>
+      <c r="B119" s="4" t="n">
+        <v>100117</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="0" t="n">
+        <v>119</v>
+      </c>
+      <c r="B120" s="4" t="n">
+        <v>100118</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="0" t="n">
+        <v>120</v>
+      </c>
+      <c r="B121" s="4" t="n">
+        <v>100119</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="0" t="n">
+        <v>121</v>
+      </c>
+      <c r="B122" s="4" t="n">
+        <v>100120</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="0" t="n">
+        <v>122</v>
+      </c>
+      <c r="B123" s="4" t="n">
+        <v>100121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[5999] Modifying the DashboardPage
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/financialTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/financialTestData.xlsx
@@ -22,12 +22,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="41">
   <si>
     <t xml:space="preserve">dataName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">voucherDate</t>
   </si>
   <si>
     <t xml:space="preserve">voucherType</t>
@@ -105,13 +102,10 @@
     <t xml:space="preserve">Public Health</t>
   </si>
   <si>
-    <t xml:space="preserve">voucherDateJune</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30/06/2016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">budgetCheck</t>
+    <t xml:space="preserve">voucherBillPayment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">budgetCheckWithSubledger</t>
   </si>
   <si>
     <t xml:space="preserve">2101001</t>
@@ -127,6 +121,15 @@
   </si>
   <si>
     <t xml:space="preserve">remittance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">budgetCheckWithOutSubledger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">voucherWithOutSubledger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">voucherWithSubledger</t>
   </si>
   <si>
     <t xml:space="preserve">bankName</t>
@@ -182,7 +185,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -204,12 +207,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <vertAlign val="superscript"/>
@@ -262,7 +259,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -272,10 +269,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -300,39 +293,38 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.1666666666667"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.4222222222222"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.4222222222222"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="20.7740740740741"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="23.2259259259259"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="43.3148148148148"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="28.6148148148148"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.2074074074074"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.62222222222222"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.6555555555556"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.2074074074074"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="21.8518518518519"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="24.3037037037037"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="45.4703703703704"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="29.9851851851852"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.1851851851852"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.01481481481481"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="0" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="0" t="s">
@@ -341,118 +333,168 @@
       <c r="G1" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="17.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="1" t="n">
+        <v>3501001</v>
+      </c>
+      <c r="E2" s="0" t="s">
         <v>10</v>
-      </c>
-      <c r="E2" s="1" t="n">
-        <v>3501001</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="0" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="3" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="n">
+        <v>2101001</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>3501003</v>
+      </c>
+      <c r="E3" s="0" t="s">
         <v>14</v>
-      </c>
-      <c r="D3" s="1" t="n">
-        <v>2101001</v>
-      </c>
-      <c r="E3" s="1" t="n">
-        <v>3501003</v>
       </c>
       <c r="F3" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="0" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="4" customFormat="false" ht="18.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>2101001</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>3501003</v>
+      </c>
+      <c r="E4" s="0" t="s">
         <v>14</v>
-      </c>
-      <c r="D4" s="1" t="n">
-        <v>2101001</v>
-      </c>
-      <c r="E4" s="1" t="n">
-        <v>3501003</v>
       </c>
       <c r="F4" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="0" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="0" t="s">
         <v>21</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" s="0" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="0" t="s">
         <v>14</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="F6" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="H6" s="0" t="n">
+      <c r="G6" s="0" t="n">
         <v>3502002</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="1" t="n">
+        <v>2101001</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>3501003</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -479,10 +521,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2296296296296"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.6444444444444"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="65.6555555555556"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.0740740740741"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.8185185185185"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="54.1888888888889"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="68.9888888888889"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.662962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -490,32 +532,32 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -542,14 +584,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7185185185185"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.2481481481481"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.8444444444444"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="30.5740740740741"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.7962962962963"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="20.7740740740741"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="22.0481481481481"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.1925925925926"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.3074074074074"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.0296296296296"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.6111111111111"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="32.1407407407407"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.7740740740741"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="21.8518518518519"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="23.0296296296296"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.5851851851852"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -557,42 +599,42 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="E1" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>15</v>
+        <v>38</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G2" s="1" t="n">
         <v>3501102</v>

</xml_diff>

<commit_message>
[5849] Modifying the Financial Page
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/financialTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/financialTestData.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="56">
   <si>
     <t xml:space="preserve">dataName</t>
   </si>
@@ -30,9 +30,18 @@
     <t xml:space="preserve">voucherType</t>
   </si>
   <si>
+    <t xml:space="preserve">fund</t>
+  </si>
+  <si>
     <t xml:space="preserve">accountCode1</t>
   </si>
   <si>
+    <t xml:space="preserve">debitAmount1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">creditAmount2</t>
+  </si>
+  <si>
     <t xml:space="preserve">accountCode2</t>
   </si>
   <si>
@@ -45,13 +54,40 @@
     <t xml:space="preserve">accountCode3</t>
   </si>
   <si>
+    <t xml:space="preserve">creditAmount3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ledgerAmount1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ledgerAmount2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ledgerType1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ledgerType2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ledgerCode1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ledgerCode2</t>
+  </si>
+  <si>
     <t xml:space="preserve">voucher1</t>
   </si>
   <si>
     <t xml:space="preserve">General</t>
   </si>
   <si>
+    <t xml:space="preserve">Municipal Fund</t>
+  </si>
+  <si>
     <t xml:space="preserve">1100101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100</t>
   </si>
   <si>
     <t xml:space="preserve">ACCOUNTS</t>
@@ -90,6 +126,12 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">contractor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G Basheer Ahmed</t>
+  </si>
+  <si>
     <t xml:space="preserve">voucher2</t>
   </si>
   <si>
@@ -123,6 +165,15 @@
     <t xml:space="preserve">remittance</t>
   </si>
   <si>
+    <t xml:space="preserve">1000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">800</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Employee</t>
+  </si>
+  <si>
     <t xml:space="preserve">budgetCheckWithOutSubledger</t>
   </si>
   <si>
@@ -153,9 +204,6 @@
     <t xml:space="preserve">ANDHRA BANK Andhra Bank RTC Busstand</t>
   </si>
   <si>
-    <t xml:space="preserve">fund</t>
-  </si>
-  <si>
     <t xml:space="preserve">billSubType</t>
   </si>
   <si>
@@ -166,9 +214,6 @@
   </si>
   <si>
     <t xml:space="preserve">expenseBill</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Municipal Fund</t>
   </si>
   <si>
     <t xml:space="preserve">3100</t>
@@ -185,7 +230,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -207,6 +252,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <vertAlign val="superscript"/>
@@ -259,7 +310,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -269,6 +320,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -293,22 +352,31 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:Q9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q13" activeCellId="0" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.6555555555556"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.2074074074074"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="21.8518518518519"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="24.3037037037037"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="45.4703703703704"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="29.9851851851852"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.1851851851852"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.3407407407407"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.6962962962963"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.3444444444444"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="22.3444444444444"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="13.1111111111111"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="14.1185185185185"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="24.8888888888889"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="46.6444444444444"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="30.7703703703704"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="20.6777777777778"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="13.5111111111111"/>
+    <col collapsed="false" hidden="false" max="13" min="12" style="1" width="14.0185185185185"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="12.1"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="11.1925925925926"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="15.837037037037"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="16.437037037037"/>
+    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="9.21111111111111"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -318,183 +386,396 @@
       <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="17.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="1" t="n">
         <v>3501001</v>
       </c>
-      <c r="E2" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>11</v>
+      <c r="H2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L2" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="M2" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="1" t="n">
         <v>2101001</v>
       </c>
-      <c r="D3" s="1" t="n">
+      <c r="E3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="1" t="n">
         <v>3501003</v>
       </c>
-      <c r="E3" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>15</v>
+      <c r="H3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L3" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="M3" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="18.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="1" t="n">
         <v>2101001</v>
       </c>
-      <c r="D4" s="1" t="n">
+      <c r="E4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="1" t="n">
         <v>3501003</v>
       </c>
-      <c r="E4" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>15</v>
+      <c r="H4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="M4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>18</v>
+        <v>27</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>21</v>
+        <v>32</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L5" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="M5" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q5" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" s="0" t="n">
+      <c r="D6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J6" s="1" t="n">
         <v>3502002</v>
       </c>
+      <c r="K6" s="1" t="n">
+        <v>200</v>
+      </c>
+      <c r="L6" s="1" t="n">
+        <v>1000</v>
+      </c>
+      <c r="M6" s="1" t="n">
+        <v>200</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q6" s="1" t="n">
+        <v>946800</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="s">
-        <v>23</v>
+      <c r="A7" s="5" t="s">
+        <v>40</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>9</v>
+        <v>27</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="0" t="s">
-        <v>21</v>
+      <c r="E7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>9</v>
+        <v>27</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="0" t="s">
-        <v>21</v>
+      <c r="E8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="1" t="n">
         <v>2101001</v>
       </c>
-      <c r="D9" s="1" t="n">
+      <c r="E9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" s="1" t="n">
         <v>3501003</v>
       </c>
-      <c r="E9" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" s="0" t="s">
-        <v>15</v>
+      <c r="H9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L9" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="M9" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q9" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -521,10 +802,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.8185185185185"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="54.1888888888889"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="68.9888888888889"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.662962962963"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.1111111111111"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.562962962963"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="70.7518518518519"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -532,32 +812,32 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -584,14 +864,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.3074074074074"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.0296296296296"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.6111111111111"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="32.1407407407407"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.7740740740741"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="21.8518518518519"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="23.0296296296296"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.5851851851852"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.6"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.4222222222222"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.5888888888889"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="32.9259259259259"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.262962962963"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="22.3444444444444"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="23.5185185185185"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.7777777777778"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -599,42 +879,42 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>33</v>
+        <v>2</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>14</v>
+        <v>19</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>28</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="G2" s="1" t="n">
         <v>3501102</v>

</xml_diff>

<commit_message>
[PHOENIX-5999] Created a method that converts the numeric to string
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/financialTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/financialTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="journalVoucherDetails" sheetId="1" state="visible" r:id="rId2"/>
@@ -399,29 +399,29 @@
   </sheetPr>
   <dimension ref="A1:Q9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q13" activeCellId="0" sqref="Q13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D:D"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.9851851851852"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.6555555555556"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.4"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="24.4"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="14.3074074074074"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="15.3851851851852"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="27.3407407407407"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="51.3481481481482"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="33.9074074074074"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="22.7333333333333"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="14.7"/>
-    <col collapsed="false" hidden="false" max="13" min="12" style="1" width="15.2888888888889"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="12.937037037037"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="12.2481481481481"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="17.2481481481481"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="17.9333333333333"/>
-    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="9.9962962962963"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.7703703703704"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.2444444444444"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.9888888888889"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="24.9888888888889"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="14.6"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="15.7777777777778"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="27.9296296296296"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="52.6222222222222"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="34.6888888888889"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="23.2259259259259"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="14.9925925925926"/>
+    <col collapsed="false" hidden="false" max="13" min="12" style="1" width="15.6777777777778"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="13.2296296296296"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="12.4444444444444"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="17.6407407407407"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="18.3259259259259"/>
+    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="10.1925925925926"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -842,15 +842,15 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+      <selection pane="topLeft" activeCell="C11" activeCellId="1" sqref="D:D C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.3851851851852"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="61.4407407407408"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="78.1"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.21111111111111"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.7777777777778"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="62.9111111111111"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="80.0592592592593"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.40740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -905,20 +905,21 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
+      <selection pane="topLeft" activeCell="H1" activeCellId="1" sqref="D:D H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.0703703703704"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.1851851851852"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.3"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.9555555555556"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.0518518518519"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="1" width="17.2481481481481"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="19.1074074074074"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="20.6777777777778"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="18.1296296296296"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.462962962963"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.6777777777778"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.9851851851852"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="12.2481481481481"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.2481481481481"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="1" width="17.6407407407407"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="19.5"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="21.1666666666667"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="18.5222222222222"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.62222222222222"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1004,20 +1005,20 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+      <selection pane="topLeft" activeCell="B12" activeCellId="1" sqref="D:D B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.4444444444444"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="20.3814814814815"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.0296296296296"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="40.2740740740741"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="45.2740740740741"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.4037037037037"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="39.6888888888889"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="46.4481481481482"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.81851851851852"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.6407407407407"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="20.8740740740741"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.4222222222222"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="41.2555555555556"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="46.4481481481482"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.7"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="40.6666666666667"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="47.5259259259259"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.01481481481481"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1102,25 +1103,25 @@
   </sheetPr>
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E18" activeCellId="1" sqref="D:D E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.7555555555556"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.8185185185185"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.1296296296296"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="15.2888888888889"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="35.6703703703704"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="8.91851851851852"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="37.9222222222222"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="1" width="12.937037037037"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="13.7185185185185"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="11.4666666666667"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="15.9740740740741"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="13.9148148148148"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.52592592592593"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="17.1481481481481"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.1111111111111"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.5222222222222"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="15.6777777777778"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="36.5518518518518"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="9.11481481481482"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="38.8074074074074"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="1" width="13.2296296296296"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="14.0148148148148"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="11.7592592592593"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="16.3666666666667"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="14.2074074074074"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.62222222222222"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>